<commit_message>
a bunch of tests ran
</commit_message>
<xml_diff>
--- a/ProjektFiler/xlsx-docs/glass.xlsx
+++ b/ProjektFiler/xlsx-docs/glass.xlsx
@@ -1,15 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="17766"/>
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\elvir\PycharmProjects\Machine_Learning_DT\ProjektFiler\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Simon\IdeaProjects\Machine_Learning_DT\ProjektFiler\xlsx-docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660"/>
+    <workbookView xWindow="240" yWindow="12" windowWidth="16092" windowHeight="9660" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="our dtc" sheetId="1" r:id="rId1"/>
@@ -63,7 +63,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -139,7 +139,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office-tema">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -214,23 +214,6 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri" panose="020F0502020204030204"/>
@@ -266,23 +249,6 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -461,19 +427,21 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F1" sqref="F1:F1048576"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultColWidth="25.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="19.796875" customWidth="1"/>
-    <col min="2" max="2" width="24.53125" customWidth="1"/>
+    <col min="1" max="1" width="19.77734375" customWidth="1"/>
+    <col min="2" max="2" width="24.5546875" customWidth="1"/>
     <col min="3" max="3" width="23" customWidth="1"/>
-    <col min="4" max="4" width="27.796875" customWidth="1"/>
+    <col min="4" max="4" width="27.77734375" customWidth="1"/>
     <col min="5" max="5" width="22" customWidth="1"/>
-    <col min="6" max="6" width="9.06640625" customWidth="1"/>
+    <col min="6" max="6" width="25.77734375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
       <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
@@ -493,7 +461,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A2" s="1">
         <v>0</v>
       </c>
@@ -527,9 +495,9 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
       <c r="B1" s="1" t="s">
         <v>6</v>
       </c>
@@ -549,7 +517,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A2" s="1">
         <v>0</v>
       </c>
@@ -581,11 +549,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G2"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
       <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
@@ -605,7 +573,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A2" s="1">
         <v>0</v>
       </c>
@@ -639,9 +607,9 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
       <c r="B1" s="1" t="s">
         <v>6</v>
       </c>
@@ -661,7 +629,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A2" s="1">
         <v>0</v>
       </c>

</xml_diff>